<commit_message>
Can load to N4j all classes and relations between them. Updated nodes properties as per ontology requirements v4.
</commit_message>
<xml_diff>
--- a/loader/src/main/resources/Units.xlsx
+++ b/loader/src/main/resources/Units.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23607"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9767ADF-1F1E-42EE-BED0-12FCA43EA4B9}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FD56218-8493-434B-A14B-9BEA72515098}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>